<commit_message>
Add chapter data retrieval to MangaOnline class and update data extraction method
</commit_message>
<xml_diff>
--- a/doc/file/lista_mangas.xlsx
+++ b/doc/file/lista_mangas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlvaroCJesus\Documents\projetos\API_de_Notifica-o_de_Mangas\doc\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86DFC14E-736B-4D2E-96A4-3F8CD4821089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD49DE7-D2F8-4851-897D-71A25F3F08E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" activeTab="1" xr2:uid="{B92754F8-F38C-4BAF-8896-4B059B5E4141}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B92754F8-F38C-4BAF-8896-4B059B5E4141}"/>
   </bookViews>
   <sheets>
     <sheet name="lista_mangas" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="318">
   <si>
     <t>url</t>
   </si>
@@ -931,6 +931,81 @@
   </si>
   <si>
     <t>home</t>
+  </si>
+  <si>
+    <t>salaryman ga isekai ni ittara shitennou ni natta hanashi</t>
+  </si>
+  <si>
+    <t>mahoutsukai no yakusou</t>
+  </si>
+  <si>
+    <t>botsuraku yotei no kizoku dakedo, hima datta kara mahou wo kiwametemita</t>
+  </si>
+  <si>
+    <t>hazure skill kinomi master: skill no mi (tabetara shinou) wo mugen ni taberareru you ni natta ken ni tsuite</t>
+  </si>
+  <si>
+    <t>izure saikyou no renkinjutsushi?</t>
+  </si>
+  <si>
+    <t>ameku takao no suiri karte</t>
+  </si>
+  <si>
+    <t>Around 40 Otoko no Isekai Tsuuhan</t>
+  </si>
+  <si>
+    <t>Solo Leveling</t>
+  </si>
+  <si>
+    <t>Sakamoto Days</t>
+  </si>
+  <si>
+    <t>Dr. Stone: Science Future</t>
+  </si>
+  <si>
+    <t>Jibaku Shounen Hanako-kun 2</t>
+  </si>
+  <si>
+    <t>Guild no Uketsukejou desu ga, Zangyou wa Iya nanode Boss wo Solo Toubatsu Shiyou to Omoimasu</t>
+  </si>
+  <si>
+    <t>Übel Blatt</t>
+  </si>
+  <si>
+    <t>Fuguushoku "Kanteishi" ga Jitsu wa Saikyou Datta</t>
+  </si>
+  <si>
+    <t>Medalist</t>
+  </si>
+  <si>
+    <t>Ishura 2nd Season</t>
+  </si>
+  <si>
+    <t>A-Rank Party wo Ridatsu shita Ore wa, Moto Oshiego-tachi to Meikyuu Shinbu wo Mezasu</t>
+  </si>
+  <si>
+    <t>Sentai Red Isekai de Boukensha ni Naru</t>
+  </si>
+  <si>
+    <t>Arifureta Shokugyou de Sekai Saikyou Season 3</t>
+  </si>
+  <si>
+    <t>Shangri-La Frontier: Kusoge Hunter, Kamige ni Idoman to su 2nd Season</t>
+  </si>
+  <si>
+    <t>Rurouni Kenshin: Meiji Kenkaku Romantan - Kyoto Douran</t>
+  </si>
+  <si>
+    <t>Kaijuu 8-gou Movie</t>
+  </si>
+  <si>
+    <t>Ninja Batman tai Yakuza League</t>
+  </si>
+  <si>
+    <t>Kaijuu 8-gou: Hoshina no Kyuujitsu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -966,37 +1041,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE97132"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE97132"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1034,8 +1085,8 @@
     <sortCondition ref="B1:B149"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CDB658B0-2032-43E1-BEAC-F06F0398078C}" uniqueName="1" name="url" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{9FC2F31E-D23D-4722-9301-838B5DE39E7C}" uniqueName="2" name="title" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{CDB658B0-2032-43E1-BEAC-F06F0398078C}" uniqueName="1" name="url" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{9FC2F31E-D23D-4722-9301-838B5DE39E7C}" uniqueName="2" name="title" queryTableFieldId="2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1379,1186 +1430,1186 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>255</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>211</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>277</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>106</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>191</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>197</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>263</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>165</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>281</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>221</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>225</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>125</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>145</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>207</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>185</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>279</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>247</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>181</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>285</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>173</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>189</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>267</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>243</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>84</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>271</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>229</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>275</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>233</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" t="s">
         <v>231</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="A50" t="s">
         <v>205</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="A51" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="A52" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="A53" t="s">
         <v>219</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
         <v>213</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="A55" t="s">
         <v>217</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="A56" t="s">
         <v>273</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="A57" t="s">
         <v>121</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" t="s">
         <v>158</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="A59" t="s">
         <v>169</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="A60" t="s">
         <v>203</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="A61" t="s">
         <v>34</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" t="s">
         <v>110</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="A63" t="s">
         <v>112</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="A64" t="s">
         <v>241</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="A65" t="s">
         <v>86</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" t="s">
         <v>92</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="A67" t="s">
         <v>187</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="A68" t="s">
         <v>239</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" t="s">
         <v>245</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="A70" t="s">
         <v>115</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="A71" t="s">
         <v>157</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="A72" t="s">
         <v>18</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="A73" t="s">
         <v>141</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
         <v>48</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="A75" t="s">
         <v>195</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
+      <c r="A76" t="s">
         <v>167</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="A77" t="s">
         <v>20</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
+      <c r="A78" t="s">
         <v>136</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="A79" t="s">
         <v>149</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="A80" t="s">
         <v>36</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="A81" t="s">
         <v>44</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="A82" t="s">
         <v>261</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="A83" t="s">
         <v>10</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="A84" t="s">
         <v>71</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="A85" t="s">
         <v>8</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
+      <c r="A86" t="s">
         <v>70</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
+      <c r="A87" t="s">
         <v>12</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="A88" t="s">
         <v>249</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
+      <c r="A89" t="s">
         <v>139</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
+      <c r="A90" t="s">
         <v>151</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" t="s">
         <v>60</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
+      <c r="A92" t="s">
         <v>16</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
+      <c r="A93" t="s">
         <v>253</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
+      <c r="A94" t="s">
         <v>38</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="A95" t="s">
         <v>259</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
+      <c r="A96" t="s">
         <v>153</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
+      <c r="A97" t="s">
         <v>108</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
+      <c r="A98" t="s">
         <v>6</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+      <c r="A99" t="s">
         <v>54</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
+      <c r="A100" t="s">
         <v>251</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="A101" t="s">
         <v>130</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="A102" t="s">
         <v>147</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
+      <c r="A103" t="s">
         <v>26</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
+      <c r="A104" t="s">
         <v>257</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
+      <c r="A105" t="s">
         <v>22</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="A106" t="s">
         <v>171</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
+      <c r="A107" t="s">
         <v>227</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
+      <c r="A108" t="s">
         <v>113</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
+      <c r="A109" t="s">
         <v>155</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
+      <c r="A110" t="s">
         <v>283</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
+      <c r="A111" t="s">
         <v>58</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
+      <c r="A112" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="A113" t="s">
         <v>52</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
+      <c r="A114" t="s">
         <v>201</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
+      <c r="A115" t="s">
         <v>163</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
+      <c r="A116" t="s">
         <v>104</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
+      <c r="A117" t="s">
         <v>179</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
+      <c r="A118" t="s">
         <v>88</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
+      <c r="A119" t="s">
         <v>199</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
+      <c r="A120" t="s">
         <v>98</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
+      <c r="A121" t="s">
         <v>161</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
+      <c r="A122" t="s">
         <v>96</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
+      <c r="A123" t="s">
         <v>68</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="A124" t="s">
         <v>40</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
+      <c r="A125" t="s">
         <v>50</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
+      <c r="A126" t="s">
         <v>127</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
+      <c r="A127" t="s">
         <v>129</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+      <c r="A128" t="s">
         <v>132</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+      <c r="A129" t="s">
         <v>133</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+      <c r="A130" t="s">
         <v>134</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="A131" t="s">
         <v>135</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
+      <c r="A132" t="s">
         <v>138</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
+      <c r="A133" t="s">
         <v>175</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
+      <c r="A134" t="s">
         <v>235</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="A135" t="s">
         <v>209</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
+      <c r="A136" t="s">
         <v>269</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
+      <c r="A137" t="s">
         <v>102</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
+      <c r="A138" t="s">
         <v>78</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+      <c r="A139" t="s">
         <v>193</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
+      <c r="A140" t="s">
         <v>94</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
+      <c r="A141" t="s">
         <v>223</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
+      <c r="A142" t="s">
         <v>265</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
+      <c r="A143" t="s">
         <v>215</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
+      <c r="A144" t="s">
         <v>119</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
+      <c r="A145" t="s">
         <v>143</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
+      <c r="A146" t="s">
         <v>183</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B146" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
+      <c r="A147" t="s">
         <v>237</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
+      <c r="A148" t="s">
         <v>42</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
+      <c r="A149" t="s">
         <v>66</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2572,10 +2623,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA1F923-E36D-41D0-8DF8-CEDE4CCE48DA}">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C173"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4221,6 +4272,267 @@
         <v>86</v>
       </c>
       <c r="C149" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>293</v>
+      </c>
+      <c r="C150" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>294</v>
+      </c>
+      <c r="B151" t="s">
+        <v>317</v>
+      </c>
+      <c r="C151" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>295</v>
+      </c>
+      <c r="B152" t="s">
+        <v>317</v>
+      </c>
+      <c r="C152" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>296</v>
+      </c>
+      <c r="B153" t="s">
+        <v>317</v>
+      </c>
+      <c r="C153" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>297</v>
+      </c>
+      <c r="B154" t="s">
+        <v>317</v>
+      </c>
+      <c r="C154" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>298</v>
+      </c>
+      <c r="B155" t="s">
+        <v>317</v>
+      </c>
+      <c r="C155" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>299</v>
+      </c>
+      <c r="B156" t="s">
+        <v>317</v>
+      </c>
+      <c r="C156" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>300</v>
+      </c>
+      <c r="B157" t="s">
+        <v>317</v>
+      </c>
+      <c r="C157" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>301</v>
+      </c>
+      <c r="B158" t="s">
+        <v>317</v>
+      </c>
+      <c r="C158" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>302</v>
+      </c>
+      <c r="B159" t="s">
+        <v>317</v>
+      </c>
+      <c r="C159" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>303</v>
+      </c>
+      <c r="B160" t="s">
+        <v>317</v>
+      </c>
+      <c r="C160" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>304</v>
+      </c>
+      <c r="B161" t="s">
+        <v>317</v>
+      </c>
+      <c r="C161" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>305</v>
+      </c>
+      <c r="B162" t="s">
+        <v>317</v>
+      </c>
+      <c r="C162" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>306</v>
+      </c>
+      <c r="B163" t="s">
+        <v>317</v>
+      </c>
+      <c r="C163" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>307</v>
+      </c>
+      <c r="B164" t="s">
+        <v>317</v>
+      </c>
+      <c r="C164" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>308</v>
+      </c>
+      <c r="B165" t="s">
+        <v>317</v>
+      </c>
+      <c r="C165" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>309</v>
+      </c>
+      <c r="B166" t="s">
+        <v>317</v>
+      </c>
+      <c r="C166" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>310</v>
+      </c>
+      <c r="B167" t="s">
+        <v>317</v>
+      </c>
+      <c r="C167" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>311</v>
+      </c>
+      <c r="B168" t="s">
+        <v>317</v>
+      </c>
+      <c r="C168" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>312</v>
+      </c>
+      <c r="B169" t="s">
+        <v>317</v>
+      </c>
+      <c r="C169" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>313</v>
+      </c>
+      <c r="B170" t="s">
+        <v>317</v>
+      </c>
+      <c r="C170" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>314</v>
+      </c>
+      <c r="B171" t="s">
+        <v>317</v>
+      </c>
+      <c r="C171" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>315</v>
+      </c>
+      <c r="B172" t="s">
+        <v>317</v>
+      </c>
+      <c r="C172" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>316</v>
+      </c>
+      <c r="B173" t="s">
+        <v>317</v>
+      </c>
+      <c r="C173" t="s">
         <v>290</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add SussyToons class for data retrieval and extraction, implement run method for execution
</commit_message>
<xml_diff>
--- a/doc/file/lista_mangas.xlsx
+++ b/doc/file/lista_mangas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlvaroCJesus\Documents\projetos\API_de_Notifica-o_de_Mangas\doc\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD49DE7-D2F8-4851-897D-71A25F3F08E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8BCC93-2F6A-4D35-B96C-E96C4F24BC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{B92754F8-F38C-4BAF-8896-4B059B5E4141}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet3!$A$1:$C$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet3!$A$1:$E$173</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">lista_mangas!$A$1:$B$149</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="336">
   <si>
     <t>url</t>
   </si>
@@ -1006,6 +1006,60 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>nome site</t>
+  </si>
+  <si>
+    <t>sussyscan</t>
+  </si>
+  <si>
+    <t>oldi.sussytoons</t>
+  </si>
+  <si>
+    <t>neoxscan</t>
+  </si>
+  <si>
+    <t>mangalivre</t>
+  </si>
+  <si>
+    <t>mangaschan</t>
+  </si>
+  <si>
+    <t>tsuki-mangas</t>
+  </si>
+  <si>
+    <t>mangaonline</t>
+  </si>
+  <si>
+    <t>disqus</t>
+  </si>
+  <si>
+    <t>jujutsuteca</t>
+  </si>
+  <si>
+    <t>lermangas</t>
+  </si>
+  <si>
+    <t>myanimelist</t>
+  </si>
+  <si>
+    <t>new.sussytoons</t>
+  </si>
+  <si>
+    <t>old.sussytoons</t>
+  </si>
+  <si>
+    <t>crunchyroll</t>
+  </si>
+  <si>
+    <t>intoxianime</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1411,9 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C4C562C-73C4-4D20-B712-CCA3369D1F1D}">
   <dimension ref="A1:B149"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B149"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2623,10 +2675,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA1F923-E36D-41D0-8DF8-CEDE4CCE48DA}">
-  <dimension ref="A1:C173"/>
+  <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E146" sqref="E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2634,9 +2686,11 @@
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2646,888 +2700,1374 @@
       <c r="C1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>324</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>212</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>324</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>278</v>
+        <v>93</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>324</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>324</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>324</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>177</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>324</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>198</v>
+        <v>103</v>
       </c>
       <c r="B12" t="s">
-        <v>197</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>324</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>264</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>263</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>324</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>324</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>319</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>282</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>281</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D16" t="s">
+        <v>319</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D17" t="s">
+        <v>319</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>222</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D18" t="s">
+        <v>319</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D19" t="s">
+        <v>319</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>225</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D20" t="s">
+        <v>319</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>319</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>319</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D23" t="s">
+        <v>319</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D24" t="s">
+        <v>319</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D25" t="s">
+        <v>319</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>186</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D26" t="s">
+        <v>319</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D27" t="s">
+        <v>319</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>280</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>279</v>
+        <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D28" t="s">
+        <v>319</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>248</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>247</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D29" t="s">
+        <v>319</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D30" t="s">
+        <v>319</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>319</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>319</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>182</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>181</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D33" t="s">
+        <v>319</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="C34" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D34" t="s">
+        <v>319</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>286</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>319</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
+        <v>288</v>
+      </c>
+      <c r="D36" t="s">
+        <v>319</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" t="s">
+        <v>288</v>
+      </c>
+      <c r="D37" t="s">
+        <v>319</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" t="s">
+        <v>288</v>
+      </c>
+      <c r="D38" t="s">
+        <v>319</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>288</v>
+      </c>
+      <c r="D39" t="s">
+        <v>319</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>288</v>
+      </c>
+      <c r="D40" t="s">
+        <v>319</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>288</v>
+      </c>
+      <c r="D41" t="s">
+        <v>319</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" t="s">
+        <v>288</v>
+      </c>
+      <c r="D42" t="s">
+        <v>319</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>288</v>
+      </c>
+      <c r="D43" t="s">
+        <v>319</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>288</v>
+      </c>
+      <c r="D44" t="s">
+        <v>319</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>288</v>
+      </c>
+      <c r="D45" t="s">
+        <v>319</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" t="s">
+        <v>288</v>
+      </c>
+      <c r="D46" t="s">
+        <v>319</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>174</v>
-      </c>
-      <c r="B38" t="s">
-        <v>173</v>
-      </c>
-      <c r="C38" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>190</v>
-      </c>
-      <c r="B39" t="s">
-        <v>189</v>
-      </c>
-      <c r="C39" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>268</v>
-      </c>
-      <c r="B40" t="s">
-        <v>267</v>
-      </c>
-      <c r="C40" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" t="s">
-        <v>72</v>
-      </c>
-      <c r="C41" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>244</v>
-      </c>
-      <c r="B42" t="s">
-        <v>243</v>
-      </c>
-      <c r="C42" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>170</v>
-      </c>
-      <c r="B43" t="s">
-        <v>169</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D47" t="s">
+        <v>320</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>168</v>
-      </c>
-      <c r="B44" t="s">
-        <v>167</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D48" t="s">
+        <v>320</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>126</v>
+      </c>
+      <c r="B49" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>272</v>
-      </c>
-      <c r="B45" t="s">
-        <v>271</v>
-      </c>
-      <c r="C45" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>230</v>
-      </c>
-      <c r="B46" t="s">
-        <v>229</v>
-      </c>
-      <c r="C46" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>276</v>
-      </c>
-      <c r="B47" t="s">
-        <v>275</v>
-      </c>
-      <c r="C47" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>234</v>
-      </c>
-      <c r="B48" t="s">
-        <v>233</v>
-      </c>
-      <c r="C48" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>232</v>
-      </c>
-      <c r="B49" t="s">
-        <v>231</v>
-      </c>
-      <c r="C49" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>320</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>146</v>
       </c>
       <c r="B50" t="s">
-        <v>205</v>
+        <v>145</v>
       </c>
       <c r="C50" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D50" t="s">
+        <v>320</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>164</v>
+        <v>122</v>
       </c>
       <c r="B51" t="s">
-        <v>163</v>
+        <v>121</v>
       </c>
       <c r="C51" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>320</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="C52" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>320</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>220</v>
+        <v>137</v>
       </c>
       <c r="B53" t="s">
-        <v>219</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D53" t="s">
+        <v>320</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>214</v>
+        <v>140</v>
       </c>
       <c r="B54" t="s">
-        <v>213</v>
+        <v>139</v>
       </c>
       <c r="C54" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D54" t="s">
+        <v>320</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>218</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>217</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D55" t="s">
+        <v>320</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>274</v>
+        <v>131</v>
       </c>
       <c r="B56" t="s">
-        <v>273</v>
+        <v>130</v>
       </c>
       <c r="C56" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D56" t="s">
+        <v>320</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D57" t="s">
+        <v>320</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C58" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D58" t="s">
+        <v>320</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>159</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>158</v>
       </c>
       <c r="C59" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D59" t="s">
+        <v>320</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="B60" t="s">
-        <v>203</v>
+        <v>157</v>
       </c>
       <c r="C60" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D60" t="s">
+        <v>320</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C61" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D61" t="s">
+        <v>320</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="C62" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D62" t="s">
+        <v>320</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="C63" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D63" t="s">
+        <v>320</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>242</v>
+        <v>154</v>
       </c>
       <c r="B64" t="s">
-        <v>241</v>
+        <v>153</v>
       </c>
       <c r="C64" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D64" t="s">
+        <v>320</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B65" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="C65" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D65" t="s">
+        <v>320</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>156</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
+        <v>155</v>
       </c>
       <c r="C66" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D66" t="s">
+        <v>320</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="B67" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D67" t="s">
+        <v>320</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>240</v>
+        <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>239</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D68" t="s">
+        <v>331</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>246</v>
+        <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>245</v>
+        <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D69" t="s">
+        <v>331</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>128</v>
       </c>
       <c r="B70" t="s">
+        <v>129</v>
+      </c>
+      <c r="C70" t="s">
+        <v>288</v>
+      </c>
+      <c r="D70" t="s">
+        <v>330</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" t="s">
+        <v>288</v>
+      </c>
+      <c r="D71" t="s">
+        <v>330</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>128</v>
+      </c>
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72" t="s">
+        <v>288</v>
+      </c>
+      <c r="D72" t="s">
+        <v>330</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>128</v>
+      </c>
+      <c r="B73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" t="s">
+        <v>288</v>
+      </c>
+      <c r="D73" t="s">
+        <v>330</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>128</v>
+      </c>
+      <c r="B74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" t="s">
+        <v>288</v>
+      </c>
+      <c r="D74" t="s">
+        <v>330</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>128</v>
+      </c>
+      <c r="B75" t="s">
         <v>138</v>
       </c>
-      <c r="C70" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>11</v>
-      </c>
-      <c r="B71" t="s">
-        <v>71</v>
-      </c>
-      <c r="C71" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>9</v>
-      </c>
-      <c r="B72" t="s">
-        <v>70</v>
-      </c>
-      <c r="C72" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>122</v>
-      </c>
-      <c r="B73" t="s">
-        <v>121</v>
-      </c>
-      <c r="C73" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>116</v>
-      </c>
-      <c r="B74" t="s">
-        <v>115</v>
-      </c>
-      <c r="C74" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>196</v>
-      </c>
-      <c r="B75" t="s">
-        <v>195</v>
-      </c>
       <c r="C75" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>330</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B76" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C76" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D76" t="s">
+        <v>330</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>256</v>
       </c>
       <c r="B77" t="s">
-        <v>139</v>
+        <v>255</v>
       </c>
       <c r="C77" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D77" t="s">
+        <v>321</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>248</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>247</v>
       </c>
       <c r="C78" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D78" t="s">
+        <v>321</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>131</v>
+        <v>244</v>
       </c>
       <c r="B79" t="s">
-        <v>130</v>
+        <v>243</v>
       </c>
       <c r="C79" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D79" t="s">
+        <v>321</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>114</v>
+        <v>240</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>239</v>
       </c>
       <c r="C80" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D80" t="s">
+        <v>321</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>246</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>245</v>
       </c>
       <c r="C81" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D81" t="s">
+        <v>321</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>262</v>
       </c>
@@ -3537,668 +4077,1034 @@
       <c r="C82" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>321</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>159</v>
+        <v>250</v>
       </c>
       <c r="B83" t="s">
-        <v>158</v>
+        <v>249</v>
       </c>
       <c r="C83" t="s">
+        <v>288</v>
+      </c>
+      <c r="D83" t="s">
+        <v>321</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" t="s">
+        <v>253</v>
+      </c>
+      <c r="C84" t="s">
+        <v>288</v>
+      </c>
+      <c r="D84" t="s">
+        <v>321</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>260</v>
+      </c>
+      <c r="B85" t="s">
+        <v>259</v>
+      </c>
+      <c r="C85" t="s">
+        <v>288</v>
+      </c>
+      <c r="D85" t="s">
+        <v>321</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>252</v>
+      </c>
+      <c r="B86" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" t="s">
+        <v>288</v>
+      </c>
+      <c r="D86" t="s">
+        <v>321</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>258</v>
+      </c>
+      <c r="B87" t="s">
+        <v>257</v>
+      </c>
+      <c r="C87" t="s">
+        <v>288</v>
+      </c>
+      <c r="D87" t="s">
+        <v>321</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>88</v>
+      </c>
+      <c r="C88" t="s">
+        <v>290</v>
+      </c>
+      <c r="D88" t="s">
+        <v>329</v>
+      </c>
+      <c r="E88" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>278</v>
+      </c>
+      <c r="B89" t="s">
+        <v>277</v>
+      </c>
+      <c r="C89" t="s">
+        <v>288</v>
+      </c>
+      <c r="D89" t="s">
+        <v>323</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>264</v>
+      </c>
+      <c r="B90" t="s">
+        <v>263</v>
+      </c>
+      <c r="C90" t="s">
+        <v>288</v>
+      </c>
+      <c r="D90" t="s">
+        <v>323</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>282</v>
+      </c>
+      <c r="B91" t="s">
+        <v>281</v>
+      </c>
+      <c r="C91" t="s">
+        <v>288</v>
+      </c>
+      <c r="D91" t="s">
+        <v>323</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>280</v>
+      </c>
+      <c r="B92" t="s">
+        <v>279</v>
+      </c>
+      <c r="C92" t="s">
+        <v>288</v>
+      </c>
+      <c r="D92" t="s">
+        <v>323</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>286</v>
+      </c>
+      <c r="B93" t="s">
+        <v>285</v>
+      </c>
+      <c r="C93" t="s">
+        <v>288</v>
+      </c>
+      <c r="D93" t="s">
+        <v>323</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>268</v>
+      </c>
+      <c r="B94" t="s">
+        <v>267</v>
+      </c>
+      <c r="C94" t="s">
+        <v>288</v>
+      </c>
+      <c r="D94" t="s">
+        <v>323</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>272</v>
+      </c>
+      <c r="B95" t="s">
+        <v>271</v>
+      </c>
+      <c r="C95" t="s">
+        <v>288</v>
+      </c>
+      <c r="D95" t="s">
+        <v>323</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>276</v>
+      </c>
+      <c r="B96" t="s">
+        <v>275</v>
+      </c>
+      <c r="C96" t="s">
+        <v>288</v>
+      </c>
+      <c r="D96" t="s">
+        <v>323</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>274</v>
+      </c>
+      <c r="B97" t="s">
+        <v>273</v>
+      </c>
+      <c r="C97" t="s">
+        <v>288</v>
+      </c>
+      <c r="D97" t="s">
+        <v>323</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>284</v>
+      </c>
+      <c r="B98" t="s">
+        <v>283</v>
+      </c>
+      <c r="C98" t="s">
+        <v>288</v>
+      </c>
+      <c r="D98" t="s">
+        <v>323</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>69</v>
+      </c>
+      <c r="B99" t="s">
+        <v>68</v>
+      </c>
+      <c r="C99" t="s">
+        <v>288</v>
+      </c>
+      <c r="D99" t="s">
+        <v>323</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>270</v>
+      </c>
+      <c r="B100" t="s">
+        <v>269</v>
+      </c>
+      <c r="C100" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100" t="s">
+        <v>323</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>266</v>
+      </c>
+      <c r="B101" t="s">
+        <v>265</v>
+      </c>
+      <c r="C101" t="s">
+        <v>288</v>
+      </c>
+      <c r="D101" t="s">
+        <v>323</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>238</v>
+      </c>
+      <c r="B102" t="s">
+        <v>237</v>
+      </c>
+      <c r="C102" t="s">
+        <v>288</v>
+      </c>
+      <c r="D102" t="s">
+        <v>323</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103" t="s">
+        <v>165</v>
+      </c>
+      <c r="C103" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>116</v>
-      </c>
-      <c r="B84" t="s">
-        <v>157</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="D103" t="s">
+        <v>325</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>85</v>
+      </c>
+      <c r="B104" t="s">
+        <v>84</v>
+      </c>
+      <c r="C104" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>142</v>
-      </c>
-      <c r="B85" t="s">
-        <v>141</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="D104" t="s">
+        <v>325</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>170</v>
+      </c>
+      <c r="B105" t="s">
+        <v>169</v>
+      </c>
+      <c r="C105" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>150</v>
-      </c>
-      <c r="B86" t="s">
-        <v>149</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="D105" t="s">
+        <v>325</v>
+      </c>
+      <c r="E105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" t="s">
+        <v>167</v>
+      </c>
+      <c r="C106" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>152</v>
-      </c>
-      <c r="B87" t="s">
-        <v>151</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="D106" t="s">
+        <v>325</v>
+      </c>
+      <c r="E106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>164</v>
+      </c>
+      <c r="B107" t="s">
+        <v>163</v>
+      </c>
+      <c r="C107" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>250</v>
-      </c>
-      <c r="B88" t="s">
-        <v>249</v>
-      </c>
-      <c r="C88" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>154</v>
-      </c>
-      <c r="B89" t="s">
-        <v>153</v>
-      </c>
-      <c r="C89" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>148</v>
-      </c>
-      <c r="B90" t="s">
-        <v>147</v>
-      </c>
-      <c r="C90" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>156</v>
-      </c>
-      <c r="B91" t="s">
-        <v>155</v>
-      </c>
-      <c r="C91" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>144</v>
-      </c>
-      <c r="B92" t="s">
-        <v>143</v>
-      </c>
-      <c r="C92" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>254</v>
-      </c>
-      <c r="B93" t="s">
-        <v>253</v>
-      </c>
-      <c r="C93" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>29</v>
-      </c>
-      <c r="B94" t="s">
-        <v>28</v>
-      </c>
-      <c r="C94" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>260</v>
-      </c>
-      <c r="B95" t="s">
-        <v>259</v>
-      </c>
-      <c r="C95" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>57</v>
-      </c>
-      <c r="B96" t="s">
-        <v>56</v>
-      </c>
-      <c r="C96" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>33</v>
-      </c>
-      <c r="B97" t="s">
-        <v>32</v>
-      </c>
-      <c r="C97" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>47</v>
-      </c>
-      <c r="B98" t="s">
-        <v>46</v>
-      </c>
-      <c r="C98" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>25</v>
-      </c>
-      <c r="B99" t="s">
-        <v>24</v>
-      </c>
-      <c r="C99" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>252</v>
-      </c>
-      <c r="B100" t="s">
-        <v>251</v>
-      </c>
-      <c r="C100" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>5</v>
-      </c>
-      <c r="B101" t="s">
-        <v>4</v>
-      </c>
-      <c r="C101" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>35</v>
-      </c>
-      <c r="B102" t="s">
-        <v>34</v>
-      </c>
-      <c r="C102" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>19</v>
-      </c>
-      <c r="B103" t="s">
-        <v>18</v>
-      </c>
-      <c r="C103" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>258</v>
-      </c>
-      <c r="B104" t="s">
-        <v>257</v>
-      </c>
-      <c r="C104" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>49</v>
-      </c>
-      <c r="B105" t="s">
-        <v>48</v>
-      </c>
-      <c r="C105" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>172</v>
-      </c>
-      <c r="B106" t="s">
-        <v>171</v>
-      </c>
-      <c r="C106" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>228</v>
-      </c>
-      <c r="B107" t="s">
-        <v>227</v>
-      </c>
-      <c r="C107" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
+        <v>325</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>21</v>
+        <v>162</v>
       </c>
       <c r="B108" t="s">
-        <v>20</v>
+        <v>161</v>
       </c>
       <c r="C108" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" t="s">
+        <v>325</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="B109" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="C109" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D109" t="s">
+        <v>325</v>
+      </c>
+      <c r="E109" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>284</v>
+        <v>111</v>
       </c>
       <c r="B110" t="s">
-        <v>283</v>
+        <v>112</v>
       </c>
       <c r="C110" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="D110" t="s">
+        <v>325</v>
+      </c>
+      <c r="E110" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>45</v>
+        <v>212</v>
       </c>
       <c r="B111" t="s">
-        <v>44</v>
+        <v>211</v>
       </c>
       <c r="C111" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D111" t="s">
+        <v>322</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>192</v>
       </c>
       <c r="B112" t="s">
-        <v>10</v>
+        <v>191</v>
       </c>
       <c r="C112" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D112" t="s">
+        <v>322</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>9</v>
+        <v>178</v>
       </c>
       <c r="B113" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="C113" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D113" t="s">
+        <v>322</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>198</v>
+      </c>
+      <c r="B114" t="s">
+        <v>197</v>
+      </c>
+      <c r="C114" t="s">
+        <v>288</v>
+      </c>
+      <c r="D114" t="s">
+        <v>322</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>222</v>
+      </c>
+      <c r="B115" t="s">
+        <v>221</v>
+      </c>
+      <c r="C115" t="s">
+        <v>288</v>
+      </c>
+      <c r="D115" t="s">
+        <v>322</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>226</v>
+      </c>
+      <c r="B116" t="s">
+        <v>225</v>
+      </c>
+      <c r="C116" t="s">
+        <v>288</v>
+      </c>
+      <c r="D116" t="s">
+        <v>322</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>208</v>
+      </c>
+      <c r="B117" t="s">
+        <v>207</v>
+      </c>
+      <c r="C117" t="s">
+        <v>288</v>
+      </c>
+      <c r="D117" t="s">
+        <v>322</v>
+      </c>
+      <c r="E117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>186</v>
+      </c>
+      <c r="B118" t="s">
+        <v>185</v>
+      </c>
+      <c r="C118" t="s">
+        <v>288</v>
+      </c>
+      <c r="D118" t="s">
+        <v>322</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>182</v>
+      </c>
+      <c r="B119" t="s">
+        <v>181</v>
+      </c>
+      <c r="C119" t="s">
+        <v>288</v>
+      </c>
+      <c r="D119" t="s">
+        <v>322</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>174</v>
+      </c>
+      <c r="B120" t="s">
+        <v>173</v>
+      </c>
+      <c r="C120" t="s">
+        <v>288</v>
+      </c>
+      <c r="D120" t="s">
+        <v>322</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>190</v>
+      </c>
+      <c r="B121" t="s">
+        <v>189</v>
+      </c>
+      <c r="C121" t="s">
+        <v>288</v>
+      </c>
+      <c r="D121" t="s">
+        <v>322</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>230</v>
+      </c>
+      <c r="B122" t="s">
+        <v>229</v>
+      </c>
+      <c r="C122" t="s">
+        <v>288</v>
+      </c>
+      <c r="D122" t="s">
+        <v>322</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>234</v>
+      </c>
+      <c r="B123" t="s">
+        <v>233</v>
+      </c>
+      <c r="C123" t="s">
+        <v>288</v>
+      </c>
+      <c r="D123" t="s">
+        <v>322</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>232</v>
+      </c>
+      <c r="B124" t="s">
+        <v>231</v>
+      </c>
+      <c r="C124" t="s">
+        <v>288</v>
+      </c>
+      <c r="D124" t="s">
+        <v>322</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>206</v>
+      </c>
+      <c r="B125" t="s">
+        <v>205</v>
+      </c>
+      <c r="C125" t="s">
+        <v>288</v>
+      </c>
+      <c r="D125" t="s">
+        <v>322</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>220</v>
+      </c>
+      <c r="B126" t="s">
+        <v>219</v>
+      </c>
+      <c r="C126" t="s">
+        <v>288</v>
+      </c>
+      <c r="D126" t="s">
+        <v>322</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>214</v>
+      </c>
+      <c r="B127" t="s">
+        <v>213</v>
+      </c>
+      <c r="C127" t="s">
+        <v>288</v>
+      </c>
+      <c r="D127" t="s">
+        <v>322</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>218</v>
+      </c>
+      <c r="B128" t="s">
+        <v>217</v>
+      </c>
+      <c r="C128" t="s">
+        <v>288</v>
+      </c>
+      <c r="D128" t="s">
+        <v>322</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>204</v>
+      </c>
+      <c r="B129" t="s">
+        <v>203</v>
+      </c>
+      <c r="C129" t="s">
+        <v>288</v>
+      </c>
+      <c r="D129" t="s">
+        <v>322</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>242</v>
+      </c>
+      <c r="B130" t="s">
+        <v>241</v>
+      </c>
+      <c r="C130" t="s">
+        <v>288</v>
+      </c>
+      <c r="D130" t="s">
+        <v>322</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>188</v>
+      </c>
+      <c r="B131" t="s">
+        <v>187</v>
+      </c>
+      <c r="C131" t="s">
+        <v>288</v>
+      </c>
+      <c r="D131" t="s">
+        <v>322</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>196</v>
+      </c>
+      <c r="B132" t="s">
+        <v>195</v>
+      </c>
+      <c r="C132" t="s">
+        <v>288</v>
+      </c>
+      <c r="D132" t="s">
+        <v>322</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>172</v>
+      </c>
+      <c r="B133" t="s">
+        <v>171</v>
+      </c>
+      <c r="C133" t="s">
+        <v>288</v>
+      </c>
+      <c r="D133" t="s">
+        <v>322</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>228</v>
+      </c>
+      <c r="B134" t="s">
+        <v>227</v>
+      </c>
+      <c r="C134" t="s">
+        <v>288</v>
+      </c>
+      <c r="D134" t="s">
+        <v>322</v>
+      </c>
+      <c r="E134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>202</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B135" t="s">
         <v>201</v>
       </c>
-      <c r="C114" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>13</v>
-      </c>
-      <c r="B115" t="s">
-        <v>12</v>
-      </c>
-      <c r="C115" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>105</v>
-      </c>
-      <c r="B116" t="s">
-        <v>104</v>
-      </c>
-      <c r="C116" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="C135" t="s">
+        <v>288</v>
+      </c>
+      <c r="D135" t="s">
+        <v>322</v>
+      </c>
+      <c r="E135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>180</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B136" t="s">
         <v>179</v>
       </c>
-      <c r="C117" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>61</v>
-      </c>
-      <c r="B118" t="s">
-        <v>60</v>
-      </c>
-      <c r="C118" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="C136" t="s">
+        <v>288</v>
+      </c>
+      <c r="D136" t="s">
+        <v>322</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>200</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B137" t="s">
         <v>199</v>
       </c>
-      <c r="C119" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>99</v>
-      </c>
-      <c r="B120" t="s">
-        <v>98</v>
-      </c>
-      <c r="C120" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>17</v>
-      </c>
-      <c r="B121" t="s">
-        <v>16</v>
-      </c>
-      <c r="C121" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>97</v>
-      </c>
-      <c r="B122" t="s">
-        <v>96</v>
-      </c>
-      <c r="C122" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>69</v>
-      </c>
-      <c r="B123" t="s">
-        <v>68</v>
-      </c>
-      <c r="C123" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>39</v>
-      </c>
-      <c r="B124" t="s">
-        <v>38</v>
-      </c>
-      <c r="C124" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>7</v>
-      </c>
-      <c r="B125" t="s">
-        <v>6</v>
-      </c>
-      <c r="C125" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>55</v>
-      </c>
-      <c r="B126" t="s">
-        <v>54</v>
-      </c>
-      <c r="C126" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>27</v>
-      </c>
-      <c r="B127" t="s">
-        <v>26</v>
-      </c>
-      <c r="C127" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>23</v>
-      </c>
-      <c r="B128" t="s">
-        <v>22</v>
-      </c>
-      <c r="C128" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>59</v>
-      </c>
-      <c r="B129" t="s">
-        <v>58</v>
-      </c>
-      <c r="C129" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>3</v>
-      </c>
-      <c r="B130" t="s">
-        <v>2</v>
-      </c>
-      <c r="C130" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>53</v>
-      </c>
-      <c r="B131" t="s">
-        <v>52</v>
-      </c>
-      <c r="C131" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>41</v>
-      </c>
-      <c r="B132" t="s">
-        <v>40</v>
-      </c>
-      <c r="C132" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="C137" t="s">
+        <v>288</v>
+      </c>
+      <c r="D137" t="s">
+        <v>322</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>176</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B138" t="s">
         <v>175</v>
       </c>
-      <c r="C133" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="C138" t="s">
+        <v>288</v>
+      </c>
+      <c r="D138" t="s">
+        <v>322</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>236</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B139" t="s">
         <v>235</v>
       </c>
-      <c r="C134" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="C139" t="s">
+        <v>288</v>
+      </c>
+      <c r="D139" t="s">
+        <v>322</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>210</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B140" t="s">
         <v>209</v>
       </c>
-      <c r="C135" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>270</v>
-      </c>
-      <c r="B136" t="s">
-        <v>269</v>
-      </c>
-      <c r="C136" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>103</v>
-      </c>
-      <c r="B137" t="s">
-        <v>102</v>
-      </c>
-      <c r="C137" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>79</v>
-      </c>
-      <c r="B138" t="s">
-        <v>78</v>
-      </c>
-      <c r="C138" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="C140" t="s">
+        <v>288</v>
+      </c>
+      <c r="D140" t="s">
+        <v>322</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>194</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B141" t="s">
         <v>193</v>
       </c>
-      <c r="C139" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>95</v>
-      </c>
-      <c r="B140" t="s">
-        <v>94</v>
-      </c>
-      <c r="C140" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="C141" t="s">
+        <v>288</v>
+      </c>
+      <c r="D141" t="s">
+        <v>322</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>224</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>223</v>
       </c>
-      <c r="C141" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>266</v>
-      </c>
-      <c r="B142" t="s">
-        <v>265</v>
-      </c>
       <c r="C142" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>322</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>216</v>
       </c>
@@ -4208,84 +5114,135 @@
       <c r="C143" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" t="s">
+        <v>322</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>51</v>
+        <v>184</v>
       </c>
       <c r="B144" t="s">
-        <v>50</v>
+        <v>183</v>
       </c>
       <c r="C144" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D144" t="s">
+        <v>322</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B145" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C145" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" t="s">
+        <v>328</v>
+      </c>
+      <c r="E145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>184</v>
+        <v>83</v>
       </c>
       <c r="B146" t="s">
-        <v>183</v>
+        <v>82</v>
       </c>
       <c r="C146" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="D146" t="s">
+        <v>327</v>
+      </c>
+      <c r="E146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>238</v>
+        <v>87</v>
       </c>
       <c r="B147" t="s">
-        <v>237</v>
+        <v>86</v>
       </c>
       <c r="C147" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="D147" t="s">
+        <v>333</v>
+      </c>
+      <c r="E147" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="B148" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="C148" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+      <c r="D148" t="s">
+        <v>326</v>
+      </c>
+      <c r="E148" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B149" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C149" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" t="s">
+        <v>332</v>
+      </c>
+      <c r="E149" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>293</v>
+        <v>294</v>
+      </c>
+      <c r="B150" t="s">
+        <v>317</v>
       </c>
       <c r="C150" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>317</v>
+      </c>
+      <c r="E150" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B151" t="s">
         <v>317</v>
@@ -4293,10 +5250,16 @@
       <c r="C151" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>317</v>
+      </c>
+      <c r="E151" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B152" t="s">
         <v>317</v>
@@ -4304,10 +5267,16 @@
       <c r="C152" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" t="s">
+        <v>317</v>
+      </c>
+      <c r="E152" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B153" t="s">
         <v>317</v>
@@ -4315,10 +5284,16 @@
       <c r="C153" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" t="s">
+        <v>317</v>
+      </c>
+      <c r="E153" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B154" t="s">
         <v>317</v>
@@ -4326,10 +5301,16 @@
       <c r="C154" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
+        <v>317</v>
+      </c>
+      <c r="E154" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B155" t="s">
         <v>317</v>
@@ -4337,10 +5318,16 @@
       <c r="C155" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>317</v>
+      </c>
+      <c r="E155" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B156" t="s">
         <v>317</v>
@@ -4348,10 +5335,16 @@
       <c r="C156" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
+        <v>317</v>
+      </c>
+      <c r="E156" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B157" t="s">
         <v>317</v>
@@ -4359,10 +5352,16 @@
       <c r="C157" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" t="s">
+        <v>317</v>
+      </c>
+      <c r="E157" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B158" t="s">
         <v>317</v>
@@ -4370,10 +5369,16 @@
       <c r="C158" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" t="s">
+        <v>317</v>
+      </c>
+      <c r="E158" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B159" t="s">
         <v>317</v>
@@ -4381,10 +5386,16 @@
       <c r="C159" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>317</v>
+      </c>
+      <c r="E159" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B160" t="s">
         <v>317</v>
@@ -4392,10 +5403,16 @@
       <c r="C160" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
+        <v>317</v>
+      </c>
+      <c r="E160" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B161" t="s">
         <v>317</v>
@@ -4403,10 +5420,16 @@
       <c r="C161" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" t="s">
+        <v>317</v>
+      </c>
+      <c r="E161" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B162" t="s">
         <v>317</v>
@@ -4414,10 +5437,16 @@
       <c r="C162" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>317</v>
+      </c>
+      <c r="E162" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B163" t="s">
         <v>317</v>
@@ -4425,10 +5454,16 @@
       <c r="C163" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" t="s">
+        <v>317</v>
+      </c>
+      <c r="E163" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B164" t="s">
         <v>317</v>
@@ -4436,10 +5471,16 @@
       <c r="C164" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
+        <v>317</v>
+      </c>
+      <c r="E164" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B165" t="s">
         <v>317</v>
@@ -4447,10 +5488,16 @@
       <c r="C165" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" t="s">
+        <v>317</v>
+      </c>
+      <c r="E165" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B166" t="s">
         <v>317</v>
@@ -4458,10 +5505,16 @@
       <c r="C166" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>317</v>
+      </c>
+      <c r="E166" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B167" t="s">
         <v>317</v>
@@ -4469,10 +5522,16 @@
       <c r="C167" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>317</v>
+      </c>
+      <c r="E167" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B168" t="s">
         <v>317</v>
@@ -4480,10 +5539,16 @@
       <c r="C168" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" t="s">
+        <v>317</v>
+      </c>
+      <c r="E168" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B169" t="s">
         <v>317</v>
@@ -4491,10 +5556,16 @@
       <c r="C169" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" t="s">
+        <v>317</v>
+      </c>
+      <c r="E169" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B170" t="s">
         <v>317</v>
@@ -4502,10 +5573,16 @@
       <c r="C170" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" t="s">
+        <v>317</v>
+      </c>
+      <c r="E170" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B171" t="s">
         <v>317</v>
@@ -4513,10 +5590,16 @@
       <c r="C171" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171" t="s">
+        <v>317</v>
+      </c>
+      <c r="E171" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B172" t="s">
         <v>317</v>
@@ -4524,22 +5607,28 @@
       <c r="C172" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" t="s">
+        <v>317</v>
+      </c>
+      <c r="E172" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>316</v>
-      </c>
-      <c r="B173" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
       <c r="C173" t="s">
         <v>290</v>
       </c>
+      <c r="E173" t="s">
+        <v>335</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C149" xr:uid="{9DA1F923-E36D-41D0-8DF8-CEDE4CCE48DA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A30:C149">
-      <sortCondition ref="B1:B149"/>
+  <autoFilter ref="A1:E173" xr:uid="{9DA1F923-E36D-41D0-8DF8-CEDE4CCE48DA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E173">
+      <sortCondition descending="1" ref="D1:D173"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>